<commit_message>
VET - Updated Monte Carlo simulations
</commit_message>
<xml_diff>
--- a/projects/va_emerging_tech/data/data_emerging_tech.xlsx
+++ b/projects/va_emerging_tech/data/data_emerging_tech.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FEB3EE-30BC-4B3A-BF1D-08FEB3120A0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A43A145-4EF7-4D05-A5AF-5BD052CA43E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="941" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connections" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="108">
   <si>
     <t>connection</t>
   </si>
@@ -243,9 +243,6 @@
     <t>BIO_TO_CCS</t>
   </si>
   <si>
-    <t>E_BIO</t>
-  </si>
-  <si>
     <t>E_BECCS</t>
   </si>
   <si>
@@ -328,9 +325,6 @@
   </si>
   <si>
     <t>NREL ATB, PV Dist Res Kansas City, moderate,2025</t>
-  </si>
-  <si>
-    <t>NREL ATB, Biomass, Dedicated, 2025</t>
   </si>
   <si>
     <t>APEN paper, incr assumed</t>
@@ -440,7 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -448,7 +442,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -906,22 +899,22 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <v>-49.2</v>
       </c>
-      <c r="M3" s="11" t="s">
-        <v>105</v>
+      <c r="M3" s="10" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -929,19 +922,19 @@
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="7">
         <v>-91.3</v>
       </c>
-      <c r="M4" s="8" t="s">
-        <v>108</v>
+      <c r="M4" s="7" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1211,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1259,7 +1252,7 @@
         <v>60</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1288,7 +1281,7 @@
         <v>45</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>61</v>
@@ -1299,13 +1292,13 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>52</v>
@@ -1322,20 +1315,20 @@
       <c r="H3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8">
+      <c r="I3" s="7"/>
+      <c r="J3" s="7">
         <v>0.23</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="7">
         <v>-2.95</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>49</v>
@@ -1355,23 +1348,23 @@
       <c r="H4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8">
+      <c r="I4" s="7"/>
+      <c r="J4" s="7">
         <v>0.95</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>53</v>
@@ -1388,22 +1381,22 @@
       <c r="H5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <v>24</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="7">
         <v>0.95</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>87</v>
+      <c r="B6" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>49</v>
@@ -1423,54 +1416,16 @@
       <c r="H6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8">
+      <c r="I6" s="7"/>
+      <c r="J6" s="7">
         <v>0.95</v>
       </c>
-      <c r="K6" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8">
-        <v>0.95</v>
-      </c>
-      <c r="K7" s="8">
+      <c r="K6" s="7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D6:I6">
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7:I7">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -1492,10 +1447,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1568,129 +1523,104 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="9">
+      <c r="A3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="8">
         <v>16.7</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="8">
+        <v>25</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8">
+        <v>30</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="7">
+        <v>90</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="7">
+        <v>66</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7">
+        <v>55</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="7">
+        <v>50</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="10">
+        <v>70</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="9">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7">
         <v>25</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9">
-        <v>30</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="8">
-        <v>90</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="8">
-        <v>66</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8">
-        <v>55</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="8">
-        <v>50</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="11">
-        <v>70</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8">
-        <v>25</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>98</v>
+      <c r="I5" s="10" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>60.6</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9">
-        <v>13500</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H6" s="10">
-        <v>45</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="9">
-        <v>60.6</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="C6" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="9">
         <f>25-3.5</f>
         <v>21.5</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="10">
+      <c r="E6" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="9">
         <v>45</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>99</v>
+      <c r="I6" s="8" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1701,10 +1631,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1801,177 +1731,145 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="8">
+      <c r="A3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="7">
         <v>1884</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>-3.15</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="7">
+        <v>14.1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>-3.15</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="13">
+        <v>2474</v>
+      </c>
+      <c r="C4" s="13">
+        <v>-0.89</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="13">
+        <v>27</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="13">
+        <v>1.59</v>
+      </c>
+      <c r="I4" s="13">
+        <v>0</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1457</v>
+      </c>
+      <c r="C5" s="13">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="7">
+        <v>16.3</v>
+      </c>
+      <c r="F5" s="13">
+        <v>-1</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="8">
-        <v>14.1</v>
-      </c>
-      <c r="F3" s="8">
-        <v>-3.15</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="H3" s="8">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8">
-        <v>0</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0.08</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="14">
-        <v>2474</v>
-      </c>
-      <c r="C4" s="14">
-        <v>-0.89</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="14">
-        <v>27</v>
-      </c>
-      <c r="F4" s="14">
-        <v>0</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="H4" s="14">
-        <v>1.59</v>
-      </c>
-      <c r="I4" s="14">
-        <v>0</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="8">
-        <v>1457</v>
-      </c>
-      <c r="C5" s="14">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E5" s="8">
-        <v>16.3</v>
-      </c>
-      <c r="F5" s="14">
-        <v>-1</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <f>9.24* 0.000001 * 277777.7778</f>
         <v>2.5666666668719995</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <v>0</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
+      <c r="J5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="10">
-        <v>4247</v>
-      </c>
-      <c r="C6" s="10">
-        <v>-0.53</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E6" s="10">
-        <v>123</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="H6" s="10">
-        <v>1.31</v>
-      </c>
-      <c r="I6" s="10">
+      <c r="B6" s="15">
+        <v>6874</v>
+      </c>
+      <c r="C6" s="9">
+        <v>-0.81</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="9">
+        <v>180.4</v>
+      </c>
+      <c r="F6" s="9">
         <v>0</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>101</v>
+      <c r="G6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="9">
+        <v>3.2</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="16">
-        <v>6874</v>
-      </c>
-      <c r="C7" s="10">
-        <v>-0.81</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="10">
-        <v>180.4</v>
-      </c>
-      <c r="F7" s="10">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" s="10">
-        <v>3.2</v>
-      </c>
-      <c r="I7" s="10">
-        <v>0</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1981,10 +1879,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2066,120 +1964,98 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8">
+        <v>80</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7">
         <v>18300</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8">
+      <c r="E3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7">
         <v>2025</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <v>2050</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="8">
+        <v>75</v>
+      </c>
+      <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H4" s="8">
+      <c r="C4" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="7">
         <v>2025</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <v>2050</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8">
+        <v>74</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7">
         <v>5200</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8">
+      <c r="E5" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7">
         <v>2025</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <v>2050</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H6" s="8">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="7">
         <v>2025</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>2050</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H7" s="8">
-        <v>2025</v>
-      </c>
-      <c r="I7" s="8">
-        <v>2050</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
va_emerging_tech - revised scenarios
</commit_message>
<xml_diff>
--- a/projects/va_emerging_tech/data/data_emerging_tech.xlsx
+++ b/projects/va_emerging_tech/data/data_emerging_tech.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A43A145-4EF7-4D05-A5AF-5BD052CA43E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95678288-4990-4EAC-AF8C-C1D9F1B588F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connections" sheetId="1" r:id="rId1"/>
@@ -456,14 +456,7 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -763,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1633,8 +1626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Re-organized va_emerging_tech and updated scenarios
</commit_message>
<xml_diff>
--- a/projects/va_emerging_tech/data/data_emerging_tech.xlsx
+++ b/projects/va_emerging_tech/data/data_emerging_tech.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F19C276-339F-4947-9DD6-E6780F24F3B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355BA1AD-5A9F-400D-8DCE-516C3E3911B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="6840" windowWidth="29040" windowHeight="15840" tabRatio="941" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="941" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connections" sheetId="1" r:id="rId1"/>
@@ -15,19 +15,10 @@
     <sheet name="PowerPlantsCosts" sheetId="10" r:id="rId5"/>
     <sheet name="PowerPlantsConstraints" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -399,9 +390,6 @@
     <t>EC_NATGAS_CCS</t>
   </si>
   <si>
-    <t>EC_PV_DIST_RES</t>
-  </si>
-  <si>
     <t>EC_BECCS</t>
   </si>
   <si>
@@ -457,6 +445,9 @@
   </si>
   <si>
     <t>fuel2</t>
+  </si>
+  <si>
+    <t>ED_PV_DIST_RES</t>
   </si>
 </sst>
 </file>
@@ -989,25 +980,25 @@
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.07421875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.4609375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.07421875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.4609375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.765625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.4609375" customWidth="1"/>
-    <col min="15" max="15" width="11.4609375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.07421875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" customWidth="1"/>
     <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1063,7 +1054,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1119,7 +1110,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -1139,7 +1130,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -1159,7 +1150,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1179,7 +1170,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -1197,15 +1188,15 @@
         <v>-163.44999999999999</v>
       </c>
       <c r="M6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
         <v>49</v>
@@ -1214,13 +1205,13 @@
         <v>99.999989999999997</v>
       </c>
       <c r="E7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P7">
         <v>2025</v>
       </c>
       <c r="R7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1237,27 +1228,27 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.4609375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.69140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.69140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.69140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.4609375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.07421875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.07421875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.23046875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.84375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1316,7 +1307,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1375,7 +1366,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1392,7 +1383,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1409,7 +1400,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1426,7 +1417,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1443,7 +1434,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1460,7 +1451,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="M13">
         <v>1</v>
       </c>
@@ -1475,22 +1466,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.3046875" customWidth="1"/>
-    <col min="4" max="4" width="12.4609375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.84375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -1498,7 +1489,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -1528,7 +1519,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
@@ -1566,7 +1557,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>106</v>
       </c>
@@ -1602,7 +1593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>105</v>
       </c>
@@ -1635,7 +1626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>104</v>
       </c>
@@ -1668,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>120</v>
       </c>
@@ -1702,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>107</v>
       </c>
@@ -1734,9 +1725,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>78</v>
@@ -1768,9 +1759,9 @@
         <v>-2.95</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>72</v>
@@ -1802,7 +1793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>108</v>
       </c>
@@ -1810,7 +1801,7 @@
         <v>118</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>52</v>
@@ -1834,9 +1825,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>49</v>
@@ -1868,7 +1859,7 @@
       </c>
       <c r="L11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>73</v>
       </c>
@@ -1904,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>109</v>
       </c>
@@ -2045,23 +2036,23 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.4609375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.4609375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -2075,7 +2066,7 @@
         <v>28</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>30</v>
@@ -2093,7 +2084,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
@@ -2125,7 +2116,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>106</v>
       </c>
@@ -2140,16 +2131,16 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I3" s="2">
         <v>15</v>
       </c>
       <c r="J3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>105</v>
       </c>
@@ -2157,7 +2148,7 @@
         <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2165,16 +2156,16 @@
         <v>12510</v>
       </c>
       <c r="H4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I4" s="2">
         <v>75</v>
       </c>
       <c r="J4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>104</v>
       </c>
@@ -2182,7 +2173,7 @@
         <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2190,16 +2181,16 @@
         <v>8700</v>
       </c>
       <c r="H5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I5" s="2">
         <v>75</v>
       </c>
       <c r="J5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>120</v>
       </c>
@@ -2225,7 +2216,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>107</v>
       </c>
@@ -2233,7 +2224,7 @@
         <v>93</v>
       </c>
       <c r="C7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2241,18 +2232,18 @@
         <v>10460</v>
       </c>
       <c r="H7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I7" s="2">
         <v>60</v>
       </c>
       <c r="J7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="B8" s="8">
         <v>16.7</v>
@@ -2276,9 +2267,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" s="8">
         <v>60.6</v>
@@ -2303,7 +2294,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>108</v>
       </c>
@@ -2311,14 +2302,14 @@
         <v>90</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D10" s="17">
         <v>100</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
@@ -2326,34 +2317,34 @@
         <v>25</v>
       </c>
       <c r="J10" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A11" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="B11" s="6">
         <v>90</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D11" s="6">
         <v>12</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I11" s="6">
         <v>30</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>73</v>
       </c>
@@ -2379,7 +2370,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>109</v>
       </c>
@@ -2394,13 +2385,13 @@
       </c>
       <c r="E13" s="6"/>
       <c r="F13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I13" s="6">
         <v>19</v>
       </c>
       <c r="J13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2414,27 +2405,27 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.07421875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.07421875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.53515625" customWidth="1"/>
-    <col min="5" max="5" width="9.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.23046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.53515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.69140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.07421875" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.5546875" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -2472,7 +2463,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -2510,7 +2501,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>106</v>
       </c>
@@ -2521,7 +2512,7 @@
         <v>-1.97</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" s="7">
         <v>25.1018404907975</v>
@@ -2530,7 +2521,7 @@
         <v>-1.97</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H3" s="7">
         <v>0</v>
@@ -2539,12 +2530,12 @@
         <v>0</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>105</v>
       </c>
@@ -2555,7 +2546,7 @@
         <v>-0.63</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E4" s="7">
         <v>58.241650294695397</v>
@@ -2564,7 +2555,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H4" s="7">
         <v>2.98</v>
@@ -2573,12 +2564,12 @@
         <v>0</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>104</v>
       </c>
@@ -2589,7 +2580,7 @@
         <v>-0.46</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E5" s="7">
         <v>56.070672261119903</v>
@@ -2598,7 +2589,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H5" s="7">
         <v>2.1890762753751201</v>
@@ -2607,12 +2598,12 @@
         <v>0</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>120</v>
       </c>
@@ -2646,7 +2637,7 @@
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>107</v>
       </c>
@@ -2657,7 +2648,7 @@
         <v>-0.73</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E7" s="7">
         <v>118.988212180746</v>
@@ -2666,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H7" s="7">
         <v>0.64396420000785803</v>
@@ -2675,14 +2666,14 @@
         <v>0</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="B8" s="7">
         <v>1884</v>
@@ -2718,9 +2709,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" s="14">
         <v>6782</v>
@@ -2738,7 +2729,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H9" s="9">
         <v>3.33</v>
@@ -2747,12 +2738,12 @@
         <v>0</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>108</v>
       </c>
@@ -2763,7 +2754,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E10" s="17">
         <v>0</v>
@@ -2778,14 +2769,14 @@
         <v>0</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B11" s="6">
         <v>5821.55</v>
@@ -2808,7 +2799,7 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>73</v>
       </c>
@@ -2843,7 +2834,7 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>109</v>
       </c>
@@ -2854,7 +2845,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E13" s="6">
         <v>70</v>
@@ -2863,7 +2854,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H13" s="6">
         <v>0</v>
@@ -2872,7 +2863,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
@@ -2887,24 +2878,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.4609375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.4609375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.07421875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.07421875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.07421875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2936,7 +2927,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -2968,7 +2959,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>106</v>
       </c>
@@ -2982,7 +2973,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>105</v>
       </c>
@@ -3002,7 +2993,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>104</v>
       </c>
@@ -3022,7 +3013,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>120</v>
       </c>
@@ -3048,7 +3039,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>107</v>
       </c>
@@ -3068,9 +3059,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -3092,9 +3083,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -3114,7 +3105,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>108</v>
       </c>
@@ -3128,9 +3119,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H11" s="7">
         <v>2025</v>
@@ -3142,7 +3133,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>73</v>
       </c>
@@ -3162,7 +3153,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>109</v>
       </c>

</xml_diff>

<commit_message>
Updated scenarios (removed H2), and set initial capacity for Transmission and Distribution
</commit_message>
<xml_diff>
--- a/projects/va_emerging_tech/data/data_emerging_tech.xlsx
+++ b/projects/va_emerging_tech/data/data_emerging_tech.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355BA1AD-5A9F-400D-8DCE-516C3E3911B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B9D798-4460-4FEF-A004-5B049FA87CE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="941" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connections" sheetId="1" r:id="rId1"/>
@@ -539,7 +539,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -559,6 +559,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -976,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1166,7 +1167,7 @@
       <c r="L5" s="10">
         <v>-49.2</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="19" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1225,7 +1226,7 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="H3" sqref="H3:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2878,7 +2879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>